<commit_message>
[Management] [Notes] Update task week 1 - November 2015. Upload Notes Vuforia.
</commit_message>
<xml_diff>
--- a/Management/Timelime.xlsx
+++ b/Management/Timelime.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Task" sheetId="1" r:id="rId1"/>
+    <sheet name="Logwork" sheetId="1" r:id="rId1"/>
     <sheet name="Bugs" sheetId="2" r:id="rId2"/>
-    <sheet name="Issues" sheetId="3" r:id="rId3"/>
+    <sheet name="PhucLS - Plan" sheetId="3" r:id="rId3"/>
+    <sheet name="PhucLS-Task" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'PhucLS-Task'!$B$2:$C$20</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Monday</t>
   </si>
@@ -121,8 +123,56 @@
     <t>ASSIGNEE</t>
   </si>
   <si>
-    <t>- Meeting with Dr. Triet, Minh.
-- Research php -&gt; asp.net (vuforia web services)</t>
+    <t>- Write services for presenter</t>
+  </si>
+  <si>
+    <t>02.11.2015</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>- .cs Page: Format to the same convention (validator, error messages,…)</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>- Research php -&gt; asp.net (vuforia web services)</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Serious</t>
+  </si>
+  <si>
+    <t>Test, Fix conflict between RequireFieldValidator and CustomValidator</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Write report =&gt; Meeting with Dr. Triet, Minh.</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>RESULT</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>- Write report for Dr. Triet.
+'- Implement Mission, Target page</t>
+  </si>
+  <si>
+    <t>- Change validator of Image type</t>
   </si>
 </sst>
 </file>
@@ -226,9 +276,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -258,6 +307,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,323 +654,325 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="27.42578125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="2" customWidth="1"/>
+    <col min="8" max="9" width="27.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="33" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="2:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -937,278 +1000,278 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="3" width="27.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="45.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="3" width="27.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1218,17 +1281,318 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="18.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="27.42578125" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="64" style="13" customWidth="1"/>
+    <col min="3" max="3" width="18" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>17</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:C20"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>